<commit_message>
adding comments to assigned papers
</commit_message>
<xml_diff>
--- a/data/egret.xlsx
+++ b/data/egret.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="28109"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/deirdreloughnan/Documents/github/egret/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/toluamuwo/Documents/WL2022/egret/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{111E263F-F2C2-C84F-A410-7ED137669736}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="660" yWindow="460" windowWidth="22540" windowHeight="15900" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="660" yWindow="460" windowWidth="22540" windowHeight="15900" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="meta_general" sheetId="2" r:id="rId1"/>
@@ -18,8 +17,14 @@
     <sheet name="data_detailed" sheetId="1" r:id="rId3"/>
     <sheet name="source_ill" sheetId="5" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
@@ -34,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12227" uniqueCount="2645">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12234" uniqueCount="2647">
   <si>
     <t>datasetID</t>
   </si>
@@ -7969,12 +7974,18 @@
   </si>
   <si>
     <t>CRD</t>
+  </si>
+  <si>
+    <t>no data to scrape</t>
+  </si>
+  <si>
+    <t>lLL needed</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -8446,38 +8457,38 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom/>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top/>
       <bottom/>
@@ -8485,7 +8496,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right/>
       <top/>
@@ -8951,10 +8962,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C72"/>
   <sheetViews>
-    <sheetView topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A46" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
       <selection activeCell="B72" sqref="B72"/>
     </sheetView>
   </sheetViews>
@@ -8969,7 +8980,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="5" t="s">
         <v>72</v>
       </c>
@@ -8983,7 +8994,7 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="6"/>
     </row>
-    <row r="5" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="6" t="s">
         <v>0</v>
       </c>
@@ -8991,7 +9002,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="6" t="s">
         <v>75</v>
       </c>
@@ -8999,7 +9010,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="6" t="s">
         <v>77</v>
       </c>
@@ -9007,7 +9018,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="6" t="s">
         <v>79</v>
       </c>
@@ -9015,7 +9026,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="6" t="s">
         <v>81</v>
       </c>
@@ -9023,7 +9034,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="6" t="s">
         <v>83</v>
       </c>
@@ -9031,7 +9042,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="6" t="s">
         <v>85</v>
       </c>
@@ -9039,7 +9050,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
         <v>87</v>
       </c>
@@ -9047,7 +9058,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="6" t="s">
         <v>89</v>
       </c>
@@ -9055,7 +9066,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
         <v>91</v>
       </c>
@@ -9063,7 +9074,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="6" t="s">
         <v>93</v>
       </c>
@@ -9071,7 +9082,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
         <v>95</v>
       </c>
@@ -9079,7 +9090,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
         <v>97</v>
       </c>
@@ -9087,7 +9098,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="6" t="s">
         <v>99</v>
       </c>
@@ -9146,7 +9157,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="6" t="s">
         <v>0</v>
       </c>
@@ -9154,7 +9165,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="6" t="s">
         <v>1</v>
       </c>
@@ -9162,7 +9173,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>2</v>
       </c>
@@ -9170,7 +9181,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="6" t="s">
         <v>3</v>
       </c>
@@ -9178,7 +9189,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="17" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="6" t="s">
         <v>4</v>
       </c>
@@ -9186,7 +9197,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="6" t="s">
         <v>5</v>
       </c>
@@ -9194,7 +9205,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
         <v>779</v>
       </c>
@@ -9202,7 +9213,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="6" t="s">
         <v>6</v>
       </c>
@@ -9210,7 +9221,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="6" t="s">
         <v>7</v>
       </c>
@@ -9218,7 +9229,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="7" t="s">
         <v>128</v>
       </c>
@@ -9226,7 +9237,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="7" t="s">
         <v>129</v>
       </c>
@@ -9234,7 +9245,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>126</v>
       </c>
@@ -9242,7 +9253,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>11</v>
       </c>
@@ -9250,7 +9261,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="7" t="s">
         <v>12</v>
       </c>
@@ -9258,7 +9269,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="42" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="7" t="s">
         <v>13</v>
       </c>
@@ -9266,7 +9277,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="7" t="s">
         <v>156</v>
       </c>
@@ -9274,7 +9285,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="44" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="7" t="s">
         <v>157</v>
       </c>
@@ -9282,7 +9293,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="45" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="7" t="s">
         <v>154</v>
       </c>
@@ -9290,7 +9301,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="46" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="7" t="s">
         <v>153</v>
       </c>
@@ -9298,7 +9309,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="47" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="7" t="s">
         <v>14</v>
       </c>
@@ -9306,7 +9317,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="48" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="7" t="s">
         <v>15</v>
       </c>
@@ -9314,7 +9325,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="49" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="7" t="s">
         <v>16</v>
       </c>
@@ -9322,7 +9333,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="50" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="7" t="s">
         <v>17</v>
       </c>
@@ -9330,7 +9341,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="51" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="7" t="s">
         <v>18</v>
       </c>
@@ -9338,7 +9349,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="52" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="7" t="s">
         <v>19</v>
       </c>
@@ -9346,7 +9357,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="53" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="7" t="s">
         <v>20</v>
       </c>
@@ -9354,7 +9365,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="54" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="7" t="s">
         <v>21</v>
       </c>
@@ -9362,7 +9373,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="55" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="7" t="s">
         <v>140</v>
       </c>
@@ -9370,7 +9381,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="56" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="7" t="s">
         <v>23</v>
       </c>
@@ -9378,7 +9389,7 @@
         <v>791</v>
       </c>
     </row>
-    <row r="57" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="7" t="s">
         <v>24</v>
       </c>
@@ -9386,7 +9397,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="7" t="s">
         <v>25</v>
       </c>
@@ -9394,7 +9405,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="7" t="s">
         <v>26</v>
       </c>
@@ -9402,7 +9413,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="60" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="7" t="s">
         <v>27</v>
       </c>
@@ -9410,7 +9421,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="61" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="7" t="s">
         <v>28</v>
       </c>
@@ -9418,7 +9429,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="62" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="7" t="s">
         <v>790</v>
       </c>
@@ -9426,7 +9437,7 @@
         <v>789</v>
       </c>
     </row>
-    <row r="63" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="7" t="s">
         <v>29</v>
       </c>
@@ -9434,7 +9445,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="7" t="s">
         <v>30</v>
       </c>
@@ -9442,7 +9453,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="65" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="7" t="s">
         <v>149</v>
       </c>
@@ -9450,7 +9461,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="66" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="7" t="s">
         <v>31</v>
       </c>
@@ -9458,7 +9469,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="67" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="7" t="s">
         <v>32</v>
       </c>
@@ -9466,7 +9477,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="68" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="7" t="s">
         <v>33</v>
       </c>
@@ -9474,7 +9485,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="69" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="7" t="s">
         <v>34</v>
       </c>
@@ -9490,7 +9501,7 @@
         <v>787</v>
       </c>
     </row>
-    <row r="71" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="7" t="s">
         <v>35</v>
       </c>
@@ -9498,7 +9509,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="72" spans="1:2" ht="17" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="7" t="s">
         <v>93</v>
       </c>
@@ -9522,10 +9533,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V488"/>
   <sheetViews>
-    <sheetView topLeftCell="H158" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="H158" workbookViewId="0">
       <selection activeCell="L179" sqref="L179"/>
     </sheetView>
   </sheetViews>
@@ -33042,7 +33053,7 @@
       <c r="T488" s="19"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:T488">
+  <sortState ref="A2:T488">
     <sortCondition ref="T2:T488"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -33050,10 +33061,10 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS267"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+    <sheetView topLeftCell="AC1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="AP1" sqref="AP1:AP1048576"/>
     </sheetView>
@@ -33064,7 +33075,7 @@
     <col min="35" max="35" width="16.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:45" ht="34" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.2">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -55587,11 +55598,11 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y483"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H154" workbookViewId="0">
-      <selection activeCell="T34" sqref="T34:T63"/>
+    <sheetView tabSelected="1" topLeftCell="F136" workbookViewId="0">
+      <selection activeCell="Q159" sqref="Q159:Q167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -64385,7 +64396,7 @@
         <v>795</v>
       </c>
       <c r="Q159" s="18" t="s">
-        <v>936</v>
+        <v>189</v>
       </c>
       <c r="R159" s="18" t="s">
         <v>276</v>
@@ -64445,7 +64456,7 @@
         <v>810</v>
       </c>
       <c r="Q160" s="18" t="s">
-        <v>225</v>
+        <v>189</v>
       </c>
       <c r="R160" s="18" t="s">
         <v>190</v>
@@ -64496,7 +64507,9 @@
       <c r="P161" s="18" t="s">
         <v>795</v>
       </c>
-      <c r="Q161" s="18"/>
+      <c r="Q161" s="18" t="s">
+        <v>189</v>
+      </c>
       <c r="R161" s="18" t="s">
         <v>227</v>
       </c>
@@ -64550,7 +64563,9 @@
       <c r="P162" s="18" t="s">
         <v>795</v>
       </c>
-      <c r="Q162" s="18"/>
+      <c r="Q162" s="18" t="s">
+        <v>2645</v>
+      </c>
       <c r="R162" s="18" t="s">
         <v>227</v>
       </c>
@@ -64606,7 +64621,9 @@
       <c r="P163" s="18" t="s">
         <v>795</v>
       </c>
-      <c r="Q163" s="18"/>
+      <c r="Q163" s="18" t="s">
+        <v>189</v>
+      </c>
       <c r="R163" s="18" t="s">
         <v>276</v>
       </c>
@@ -64662,7 +64679,9 @@
       <c r="P164" s="18" t="s">
         <v>795</v>
       </c>
-      <c r="Q164" s="18"/>
+      <c r="Q164" s="18" t="s">
+        <v>189</v>
+      </c>
       <c r="R164" s="18" t="s">
         <v>38</v>
       </c>
@@ -64714,7 +64733,9 @@
       <c r="P165" s="18" t="s">
         <v>795</v>
       </c>
-      <c r="Q165" s="18"/>
+      <c r="Q165" s="18" t="s">
+        <v>189</v>
+      </c>
       <c r="R165" s="18" t="s">
         <v>38</v>
       </c>
@@ -64768,7 +64789,9 @@
       <c r="P166" s="18" t="s">
         <v>795</v>
       </c>
-      <c r="Q166" s="18"/>
+      <c r="Q166" s="18" t="s">
+        <v>189</v>
+      </c>
       <c r="R166" s="18" t="s">
         <v>276</v>
       </c>
@@ -64824,7 +64847,9 @@
       <c r="P167" s="18" t="s">
         <v>795</v>
       </c>
-      <c r="Q167" s="18"/>
+      <c r="Q167" s="18" t="s">
+        <v>2646</v>
+      </c>
       <c r="R167" s="18" t="s">
         <v>276</v>
       </c>
@@ -72386,7 +72411,7 @@
       <c r="C483" s="18"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U167">
+  <sortState ref="A2:U167">
     <sortCondition ref="T2:T167"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CRD papers update on availability or rejection
</commit_message>
<xml_diff>
--- a/data/egret.xlsx
+++ b/data/egret.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/christophe_rouleau-desrochers/Documents/github/egret/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CB9228D-1CA3-3D45-AC0D-6C533E6A5645}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAF658DC-0F21-614F-B8E5-857573D78650}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="29400" windowHeight="18400" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="29400" yWindow="-1620" windowWidth="38400" windowHeight="21600" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_general" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12234" uniqueCount="2647">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12281" uniqueCount="2648">
   <si>
     <t>datasetID</t>
   </si>
@@ -7981,6 +7981,9 @@
   </si>
   <si>
     <t>lLL needed</t>
+  </si>
+  <si>
+    <t>not in english</t>
   </si>
 </sst>
 </file>
@@ -9527,7 +9530,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:V488"/>
   <sheetViews>
-    <sheetView topLeftCell="H158" workbookViewId="0">
+    <sheetView topLeftCell="D75" workbookViewId="0">
       <selection activeCell="L179" sqref="L179"/>
     </sheetView>
   </sheetViews>
@@ -33026,9 +33029,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:AS267"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A146" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AP1" sqref="AP1:AP1048576"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AK196" sqref="AK196"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -55563,8 +55566,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U451"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="S53" sqref="S53"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="150" workbookViewId="0">
+      <selection activeCell="N46" sqref="N46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -57232,6 +57235,12 @@
       <c r="K34" t="s">
         <v>188</v>
       </c>
+      <c r="L34" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M34" t="s">
+        <v>2647</v>
+      </c>
       <c r="P34" t="s">
         <v>795</v>
       </c>
@@ -57279,6 +57288,12 @@
       <c r="K35" t="s">
         <v>188</v>
       </c>
+      <c r="L35" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M35" t="s">
+        <v>2647</v>
+      </c>
       <c r="R35" t="s">
         <v>276</v>
       </c>
@@ -57323,6 +57338,12 @@
       <c r="K36" t="s">
         <v>188</v>
       </c>
+      <c r="L36" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M36" t="s">
+        <v>2647</v>
+      </c>
       <c r="R36" t="s">
         <v>227</v>
       </c>
@@ -57370,6 +57391,12 @@
       <c r="K37" t="s">
         <v>188</v>
       </c>
+      <c r="L37" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M37" t="s">
+        <v>2647</v>
+      </c>
       <c r="R37" t="s">
         <v>227</v>
       </c>
@@ -57417,6 +57444,12 @@
       <c r="K38" t="s">
         <v>188</v>
       </c>
+      <c r="L38" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M38" t="s">
+        <v>2647</v>
+      </c>
       <c r="R38" t="s">
         <v>227</v>
       </c>
@@ -57464,6 +57497,12 @@
       <c r="K39" t="s">
         <v>188</v>
       </c>
+      <c r="L39" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M39" t="s">
+        <v>2647</v>
+      </c>
       <c r="R39" t="s">
         <v>227</v>
       </c>
@@ -57511,6 +57550,12 @@
       <c r="K40" t="s">
         <v>188</v>
       </c>
+      <c r="L40" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M40" t="s">
+        <v>2647</v>
+      </c>
       <c r="P40" t="s">
         <v>42</v>
       </c>
@@ -57561,6 +57606,12 @@
       <c r="K41" t="s">
         <v>188</v>
       </c>
+      <c r="L41" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M41" t="s">
+        <v>2647</v>
+      </c>
       <c r="P41" t="s">
         <v>42</v>
       </c>
@@ -57605,6 +57656,12 @@
       <c r="K42" t="s">
         <v>188</v>
       </c>
+      <c r="L42" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M42" t="s">
+        <v>2647</v>
+      </c>
       <c r="P42" t="s">
         <v>2158</v>
       </c>
@@ -57655,6 +57712,12 @@
       <c r="K43" t="s">
         <v>188</v>
       </c>
+      <c r="L43" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M43" t="s">
+        <v>2647</v>
+      </c>
       <c r="R43" t="s">
         <v>333</v>
       </c>
@@ -57699,6 +57762,12 @@
       <c r="K44" t="s">
         <v>188</v>
       </c>
+      <c r="L44" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M44" t="s">
+        <v>2647</v>
+      </c>
       <c r="P44" t="s">
         <v>42</v>
       </c>
@@ -57749,6 +57818,12 @@
       <c r="K45" t="s">
         <v>188</v>
       </c>
+      <c r="L45" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M45" t="s">
+        <v>2647</v>
+      </c>
       <c r="N45" t="s">
         <v>189</v>
       </c>
@@ -57802,6 +57877,12 @@
       <c r="K46" t="s">
         <v>188</v>
       </c>
+      <c r="L46" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M46" t="s">
+        <v>2647</v>
+      </c>
       <c r="N46" t="s">
         <v>821</v>
       </c>
@@ -57855,6 +57936,12 @@
       <c r="K47" t="s">
         <v>188</v>
       </c>
+      <c r="L47" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M47" t="s">
+        <v>2647</v>
+      </c>
       <c r="P47" t="s">
         <v>795</v>
       </c>
@@ -57902,6 +57989,9 @@
       <c r="K48" t="s">
         <v>188</v>
       </c>
+      <c r="N48" t="s">
+        <v>642</v>
+      </c>
       <c r="P48" t="s">
         <v>795</v>
       </c>
@@ -57952,6 +58042,12 @@
       <c r="K49" t="s">
         <v>188</v>
       </c>
+      <c r="L49" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M49" t="s">
+        <v>2647</v>
+      </c>
       <c r="P49" t="s">
         <v>795</v>
       </c>
@@ -58002,6 +58098,12 @@
       <c r="K50" t="s">
         <v>188</v>
       </c>
+      <c r="L50" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M50" t="s">
+        <v>2647</v>
+      </c>
       <c r="P50" t="s">
         <v>795</v>
       </c>
@@ -58052,6 +58154,9 @@
       <c r="K51" t="s">
         <v>188</v>
       </c>
+      <c r="N51" t="s">
+        <v>189</v>
+      </c>
       <c r="P51" t="s">
         <v>844</v>
       </c>
@@ -58103,7 +58208,7 @@
         <v>188</v>
       </c>
       <c r="N52" t="s">
-        <v>189</v>
+        <v>642</v>
       </c>
       <c r="P52" t="s">
         <v>795</v>
@@ -58155,6 +58260,9 @@
       <c r="K53" t="s">
         <v>188</v>
       </c>
+      <c r="N53" t="s">
+        <v>642</v>
+      </c>
       <c r="P53" t="s">
         <v>795</v>
       </c>
@@ -58199,6 +58307,9 @@
       <c r="K54" t="s">
         <v>188</v>
       </c>
+      <c r="N54" t="s">
+        <v>189</v>
+      </c>
       <c r="P54" t="s">
         <v>795</v>
       </c>
@@ -58246,6 +58357,9 @@
       <c r="K55" t="s">
         <v>188</v>
       </c>
+      <c r="N55" t="s">
+        <v>642</v>
+      </c>
       <c r="P55" t="s">
         <v>795</v>
       </c>
@@ -58296,6 +58410,9 @@
       <c r="K56" t="s">
         <v>188</v>
       </c>
+      <c r="N56" t="s">
+        <v>642</v>
+      </c>
       <c r="P56" t="s">
         <v>795</v>
       </c>
@@ -58346,6 +58463,9 @@
       <c r="K57" t="s">
         <v>188</v>
       </c>
+      <c r="N57" t="s">
+        <v>642</v>
+      </c>
       <c r="P57" t="s">
         <v>795</v>
       </c>
@@ -58396,6 +58516,12 @@
       <c r="K58" t="s">
         <v>188</v>
       </c>
+      <c r="L58" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M58" t="s">
+        <v>2647</v>
+      </c>
       <c r="R58" t="s">
         <v>227</v>
       </c>
@@ -58443,6 +58569,9 @@
       <c r="K59" t="s">
         <v>188</v>
       </c>
+      <c r="N59" t="s">
+        <v>189</v>
+      </c>
       <c r="P59" t="s">
         <v>47</v>
       </c>
@@ -58493,6 +58622,9 @@
       <c r="K60" t="s">
         <v>188</v>
       </c>
+      <c r="N60" t="s">
+        <v>642</v>
+      </c>
       <c r="P60" t="s">
         <v>795</v>
       </c>
@@ -58540,6 +58672,9 @@
       <c r="K61" t="s">
         <v>188</v>
       </c>
+      <c r="N61" t="s">
+        <v>189</v>
+      </c>
       <c r="P61" t="s">
         <v>795</v>
       </c>
@@ -58590,6 +58725,12 @@
       <c r="K62" t="s">
         <v>188</v>
       </c>
+      <c r="L62" t="s">
+        <v>2647</v>
+      </c>
+      <c r="M62" t="s">
+        <v>2647</v>
+      </c>
       <c r="P62" t="s">
         <v>795</v>
       </c>
@@ -58639,6 +58780,9 @@
       </c>
       <c r="K63" t="s">
         <v>188</v>
+      </c>
+      <c r="N63" t="s">
+        <v>189</v>
       </c>
       <c r="P63" t="s">
         <v>795</v>

</xml_diff>

<commit_message>
data scraping + progress update
</commit_message>
<xml_diff>
--- a/data/egret.xlsx
+++ b/data/egret.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17782\Documents\GitHub\egret\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D97741-AB62-42BF-8A2A-2F7E6D64D26D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F702FA88-5F19-4316-A44A-E5B9D65A2FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12281" uniqueCount="2652">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12281" uniqueCount="2653">
   <si>
     <t>datasetID</t>
   </si>
@@ -7996,6 +7996,9 @@
   </si>
   <si>
     <t>unavailable</t>
+  </si>
+  <si>
+    <t>ask BW/JN</t>
   </si>
 </sst>
 </file>
@@ -55578,8 +55581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U451"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="S89" sqref="S89"/>
+    <sheetView tabSelected="1" topLeftCell="M85" zoomScale="150" workbookViewId="0">
+      <selection activeCell="V92" sqref="V92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -59703,7 +59706,7 @@
         <v>276</v>
       </c>
       <c r="U81" t="s">
-        <v>42</v>
+        <v>2652</v>
       </c>
     </row>
     <row r="82" spans="1:21" x14ac:dyDescent="0.3">
@@ -59753,7 +59756,7 @@
         <v>276</v>
       </c>
       <c r="U82" t="s">
-        <v>42</v>
+        <v>2652</v>
       </c>
     </row>
     <row r="83" spans="1:21" x14ac:dyDescent="0.3">
@@ -59803,7 +59806,7 @@
         <v>276</v>
       </c>
       <c r="U83" t="s">
-        <v>42</v>
+        <v>2652</v>
       </c>
     </row>
     <row r="84" spans="1:21" x14ac:dyDescent="0.3">
@@ -59906,7 +59909,7 @@
         <v>276</v>
       </c>
       <c r="U85" t="s">
-        <v>42</v>
+        <v>2650</v>
       </c>
     </row>
     <row r="86" spans="1:21" x14ac:dyDescent="0.3">
@@ -59956,7 +59959,7 @@
         <v>276</v>
       </c>
       <c r="U86" t="s">
-        <v>42</v>
+        <v>2652</v>
       </c>
     </row>
     <row r="87" spans="1:21" x14ac:dyDescent="0.3">
@@ -60053,7 +60056,7 @@
         <v>276</v>
       </c>
       <c r="U88" t="s">
-        <v>42</v>
+        <v>2648</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
data scraping + update progress
</commit_message>
<xml_diff>
--- a/data/egret.xlsx
+++ b/data/egret.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17782\Documents\GitHub\egret\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F702FA88-5F19-4316-A44A-E5B9D65A2FF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE6F6D04-41EB-48F6-A18D-8467B43665DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -55581,8 +55581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:U451"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M85" zoomScale="150" workbookViewId="0">
-      <selection activeCell="V92" sqref="V92"/>
+    <sheetView tabSelected="1" topLeftCell="M73" zoomScale="150" workbookViewId="0">
+      <selection activeCell="U98" sqref="U98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -60388,7 +60388,7 @@
         <v>276</v>
       </c>
       <c r="U95" t="s">
-        <v>42</v>
+        <v>2648</v>
       </c>
     </row>
     <row r="96" spans="1:21" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
undoing changes to main data file
</commit_message>
<xml_diff>
--- a/data/egret.xlsx
+++ b/data/egret.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sapph\Documents\ubc things\work\egret\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\17782\Documents\GitHub\egret\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDDC59F5-A263-4FCE-8285-5768B11E0014}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C14CE382-C730-4C8E-A284-80316910A347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="meta_general" sheetId="2" r:id="rId1"/>
@@ -8499,9 +8499,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Office 2013 - 2022">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -8539,7 +8539,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office 2013 - 2022">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -8645,7 +8645,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office 2013 - 2022">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -8787,7 +8787,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -9368,8 +9368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:U488"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A323" workbookViewId="0">
-      <selection activeCell="C342" sqref="C342"/>
+    <sheetView tabSelected="1" topLeftCell="G304" workbookViewId="0">
+      <selection activeCell="L204" sqref="L204"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -9382,7 +9382,7 @@
     <col min="19" max="19" width="13.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>134</v>
       </c>
@@ -9444,7 +9444,7 @@
         <v>740</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>296</v>
       </c>
@@ -9482,7 +9482,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>149</v>
       </c>
@@ -9526,7 +9526,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -9573,7 +9573,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>149</v>
       </c>
@@ -9620,7 +9620,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>149</v>
       </c>
@@ -9670,7 +9670,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>149</v>
       </c>
@@ -9720,7 +9720,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>149</v>
       </c>
@@ -9767,7 +9767,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>149</v>
       </c>
@@ -9817,7 +9817,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>149</v>
       </c>
@@ -9864,7 +9864,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>149</v>
       </c>
@@ -9911,7 +9911,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>149</v>
       </c>
@@ -9958,7 +9958,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>149</v>
       </c>
@@ -10005,7 +10005,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>149</v>
       </c>
@@ -10055,7 +10055,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>149</v>
       </c>
@@ -10102,7 +10102,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>149</v>
       </c>
@@ -10149,7 +10149,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>149</v>
       </c>
@@ -10196,7 +10196,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>149</v>
       </c>
@@ -10246,7 +10246,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>149</v>
       </c>
@@ -10296,7 +10296,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>149</v>
       </c>
@@ -10343,7 +10343,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>149</v>
       </c>
@@ -10390,7 +10390,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>149</v>
       </c>
@@ -10437,7 +10437,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>149</v>
       </c>
@@ -10490,7 +10490,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>149</v>
       </c>
@@ -10537,7 +10537,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>149</v>
       </c>
@@ -10584,7 +10584,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>149</v>
       </c>
@@ -10634,7 +10634,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>149</v>
       </c>
@@ -10681,7 +10681,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>149</v>
       </c>
@@ -10728,7 +10728,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>149</v>
       </c>
@@ -10778,7 +10778,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>149</v>
       </c>
@@ -34271,7 +34271,7 @@
     <col min="1" max="1" width="13.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A1" s="13" t="s">
         <v>134</v>
       </c>
@@ -34336,7 +34336,7 @@
         <v>2597</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>149</v>
       </c>
@@ -34383,7 +34383,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>149</v>
       </c>
@@ -34433,7 +34433,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>149</v>
       </c>
@@ -34480,7 +34480,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>149</v>
       </c>
@@ -34527,7 +34527,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>149</v>
       </c>
@@ -34577,7 +34577,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>149</v>
       </c>
@@ -34627,7 +34627,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>149</v>
       </c>
@@ -34677,7 +34677,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>149</v>
       </c>
@@ -34724,7 +34724,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>149</v>
       </c>
@@ -34771,7 +34771,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>149</v>
       </c>
@@ -34821,7 +34821,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>149</v>
       </c>
@@ -34871,7 +34871,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>149</v>
       </c>
@@ -34921,7 +34921,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>149</v>
       </c>
@@ -34971,7 +34971,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>149</v>
       </c>
@@ -35021,7 +35021,7 @@
         <v>2602</v>
       </c>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>149</v>
       </c>
@@ -35071,7 +35071,7 @@
         <v>2599</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>337</v>
       </c>
@@ -35115,7 +35115,7 @@
         <v>2599</v>
       </c>
     </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>149</v>
       </c>
@@ -35162,7 +35162,7 @@
         <v>2599</v>
       </c>
     </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>149</v>
       </c>
@@ -35209,7 +35209,7 @@
         <v>2599</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>149</v>
       </c>
@@ -35259,7 +35259,7 @@
         <v>2599</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>149</v>
       </c>
@@ -35306,7 +35306,7 @@
         <v>2599</v>
       </c>
     </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>149</v>
       </c>
@@ -35356,7 +35356,7 @@
         <v>2599</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>149</v>
       </c>
@@ -35406,7 +35406,7 @@
         <v>2599</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>149</v>
       </c>
@@ -35459,7 +35459,7 @@
         <v>2599</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>149</v>
       </c>
@@ -35512,7 +35512,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>149</v>
       </c>
@@ -35565,7 +35565,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>149</v>
       </c>
@@ -35609,7 +35609,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>149</v>
       </c>
@@ -35656,7 +35656,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>149</v>
       </c>
@@ -35706,7 +35706,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>296</v>
       </c>
@@ -35750,7 +35750,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>149</v>
       </c>
@@ -35797,7 +35797,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>149</v>
       </c>
@@ -35847,7 +35847,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>149</v>
       </c>
@@ -35897,7 +35897,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>149</v>
       </c>
@@ -35953,7 +35953,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>149</v>
       </c>
@@ -36003,7 +36003,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>149</v>
       </c>
@@ -36053,7 +36053,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -36106,7 +36106,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>149</v>
       </c>
@@ -36159,7 +36159,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>149</v>
       </c>
@@ -36212,7 +36212,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>149</v>
       </c>
@@ -36268,7 +36268,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>149</v>
       </c>
@@ -36324,7 +36324,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>149</v>
       </c>
@@ -36374,7 +36374,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>149</v>
       </c>
@@ -36427,7 +36427,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>149</v>
       </c>
@@ -36480,7 +36480,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>149</v>
       </c>
@@ -36539,7 +36539,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>149</v>
       </c>
@@ -36598,7 +36598,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>149</v>
       </c>
@@ -36654,7 +36654,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>149</v>
       </c>
@@ -36704,7 +36704,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>149</v>
       </c>
@@ -36760,7 +36760,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>149</v>
       </c>
@@ -36816,7 +36816,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>149</v>
       </c>
@@ -36869,7 +36869,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>149</v>
       </c>
@@ -36922,7 +36922,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>149</v>
       </c>
@@ -36975,7 +36975,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>335</v>
       </c>
@@ -37022,7 +37022,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>149</v>
       </c>
@@ -37072,7 +37072,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>149</v>
       </c>
@@ -37125,7 +37125,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>149</v>
       </c>
@@ -37284,7 +37284,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>149</v>
       </c>
@@ -37337,7 +37337,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>149</v>
       </c>
@@ -37387,7 +37387,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>149</v>
       </c>
@@ -37443,7 +37443,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>149</v>
       </c>
@@ -37496,7 +37496,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>149</v>
       </c>
@@ -37546,7 +37546,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>149</v>
       </c>
@@ -37596,7 +37596,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>149</v>
       </c>
@@ -37646,7 +37646,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>149</v>
       </c>
@@ -37693,7 +37693,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>149</v>
       </c>
@@ -37737,7 +37737,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>149</v>
       </c>
@@ -37787,7 +37787,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>149</v>
       </c>
@@ -37837,7 +37837,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>149</v>
       </c>
@@ -37937,7 +37937,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>149</v>
       </c>
@@ -37987,7 +37987,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>149</v>
       </c>
@@ -38037,7 +38037,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>149</v>
       </c>
@@ -38087,7 +38087,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>149</v>
       </c>
@@ -38137,7 +38137,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>149</v>
       </c>
@@ -38187,7 +38187,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>149</v>
       </c>
@@ -38240,7 +38240,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>149</v>
       </c>
@@ -38290,7 +38290,7 @@
         <v>2606</v>
       </c>
     </row>
-    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>149</v>
       </c>
@@ -38340,7 +38340,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>149</v>
       </c>
@@ -38390,7 +38390,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>149</v>
       </c>
@@ -38440,7 +38440,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>149</v>
       </c>
@@ -38490,7 +38490,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>149</v>
       </c>
@@ -38543,7 +38543,7 @@
         <v>2606</v>
       </c>
     </row>
-    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>149</v>
       </c>
@@ -38593,7 +38593,7 @@
         <v>2608</v>
       </c>
     </row>
-    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>149</v>
       </c>
@@ -38643,7 +38643,7 @@
         <v>2610</v>
       </c>
     </row>
-    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>149</v>
       </c>
@@ -38693,7 +38693,7 @@
         <v>2609</v>
       </c>
     </row>
-    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>335</v>
       </c>
@@ -38740,7 +38740,7 @@
         <v>2606</v>
       </c>
     </row>
-    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>285</v>
       </c>
@@ -38787,7 +38787,7 @@
         <v>2608</v>
       </c>
     </row>
-    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>149</v>
       </c>
@@ -38837,7 +38837,7 @@
         <v>2608</v>
       </c>
     </row>
-    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>149</v>
       </c>
@@ -38884,7 +38884,7 @@
         <v>2608</v>
       </c>
     </row>
-    <row r="92" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>149</v>
       </c>
@@ -38931,7 +38931,7 @@
         <v>2606</v>
       </c>
     </row>
-    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>149</v>
       </c>
@@ -38978,7 +38978,7 @@
         <v>2608</v>
       </c>
     </row>
-    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>149</v>
       </c>
@@ -39025,7 +39025,7 @@
         <v>2607</v>
       </c>
     </row>
-    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>149</v>
       </c>
@@ -39072,7 +39072,7 @@
         <v>2606</v>
       </c>
     </row>
-    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:21" ht="16.05" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>149</v>
       </c>

</xml_diff>